<commit_message>
- hero name is always visible, when is not empty
</commit_message>
<xml_diff>
--- a/hero_properties.xlsx
+++ b/hero_properties.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Life</t>
   </si>
@@ -66,9 +66,6 @@
     <t>sec</t>
   </si>
   <si>
-    <t>fire ball</t>
-  </si>
-  <si>
     <t>fire bomb</t>
   </si>
   <si>
@@ -84,19 +81,31 @@
     <t>thunder bolt</t>
   </si>
   <si>
-    <t>thunder missle</t>
-  </si>
-  <si>
     <t>black fire</t>
   </si>
   <si>
     <t>skull</t>
   </si>
   <si>
-    <t>blue missle</t>
-  </si>
-  <si>
-    <t>red missle</t>
+    <t>Mana Consumed</t>
+  </si>
+  <si>
+    <t>frost fury</t>
+  </si>
+  <si>
+    <t>electric shock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fire </t>
+  </si>
+  <si>
+    <t>lightning</t>
+  </si>
+  <si>
+    <t>electric bomb</t>
+  </si>
+  <si>
+    <t>bloody whip</t>
   </si>
 </sst>
 </file>
@@ -555,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R10"/>
+  <dimension ref="A2:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,16 +577,16 @@
     <col min="8" max="8" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" customWidth="1"/>
     <col min="10" max="10" width="12.44140625" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" customWidth="1"/>
-    <col min="15" max="15" width="13.21875" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" customWidth="1"/>
-    <col min="17" max="17" width="14.21875" customWidth="1"/>
+    <col min="11" max="12" width="13.44140625" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" customWidth="1"/>
+    <col min="16" max="16" width="13.21875" customWidth="1"/>
+    <col min="17" max="18" width="13.33203125" customWidth="1"/>
+    <col min="19" max="19" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="6" t="s">
@@ -603,35 +612,42 @@
       <c r="K2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="L2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="R2" s="9"/>
+      <c r="R2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="9"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -649,10 +665,10 @@
         <v>200</v>
       </c>
       <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4">
         <v>16</v>
-      </c>
-      <c r="I4">
-        <v>10</v>
       </c>
       <c r="J4">
         <v>0.2</v>
@@ -660,11 +676,26 @@
       <c r="K4">
         <v>3</v>
       </c>
-      <c r="M4" t="s">
-        <v>17</v>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="N4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4">
+        <v>24</v>
+      </c>
+      <c r="P4">
+        <v>0.25</v>
+      </c>
+      <c r="Q4">
+        <v>6</v>
+      </c>
+      <c r="R4">
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -682,13 +713,37 @@
         <v>186.66666666666669</v>
       </c>
       <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5">
+        <v>14</v>
+      </c>
+      <c r="J5">
+        <v>0.2</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+      <c r="N5" t="s">
         <v>19</v>
       </c>
-      <c r="M5" t="s">
-        <v>20</v>
+      <c r="O5">
+        <v>21</v>
+      </c>
+      <c r="P5">
+        <v>0.25</v>
+      </c>
+      <c r="Q5">
+        <v>6</v>
+      </c>
+      <c r="R5">
+        <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -706,13 +761,37 @@
         <v>168.84615384615384</v>
       </c>
       <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6">
+        <v>15</v>
+      </c>
+      <c r="J6">
+        <v>0.2</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="N6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6">
         <v>22</v>
       </c>
-      <c r="M6" t="s">
-        <v>21</v>
+      <c r="P6">
+        <v>0.25</v>
+      </c>
+      <c r="Q6">
+        <v>6</v>
+      </c>
+      <c r="R6">
+        <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -730,13 +809,37 @@
         <v>170</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="I8">
+        <v>12</v>
+      </c>
+      <c r="J8">
+        <v>0.25</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>10</v>
+      </c>
+      <c r="N8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8">
+        <v>18</v>
+      </c>
+      <c r="P8">
+        <v>0.3</v>
+      </c>
+      <c r="Q8">
+        <v>8</v>
+      </c>
+      <c r="R8">
+        <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -756,11 +859,35 @@
       <c r="H9" t="s">
         <v>25</v>
       </c>
-      <c r="M9" t="s">
-        <v>26</v>
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>0.25</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>10</v>
+      </c>
+      <c r="N9" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9">
+        <v>16</v>
+      </c>
+      <c r="P9">
+        <v>0.3</v>
+      </c>
+      <c r="Q9">
+        <v>8</v>
+      </c>
+      <c r="R9">
+        <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -776,6 +903,36 @@
       <c r="F10">
         <f t="shared" si="0"/>
         <v>165</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10">
+        <v>13</v>
+      </c>
+      <c r="J10">
+        <v>0.25</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>10</v>
+      </c>
+      <c r="N10" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10">
+        <v>20</v>
+      </c>
+      <c r="P10">
+        <v>0.3</v>
+      </c>
+      <c r="Q10">
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>